<commit_message>
next float with edge case.
</commit_message>
<xml_diff>
--- a/docs/ULP.xlsx
+++ b/docs/ULP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ushio\Documents\RayTracing\of_v0.10.1_vs2017_release\apps\with_ogaki\study\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B8FDC4-38BB-40D7-BFB1-27423FCF2445}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756BE9C9-511C-4C9C-AB5B-118D9C7C758A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4568" yWindow="487" windowWidth="23872" windowHeight="15188" xr2:uid="{ECB7C8CB-0843-4239-9044-DBF34DC2D882}"/>
+    <workbookView xWindow="232" yWindow="4298" windowWidth="23873" windowHeight="15187" xr2:uid="{ECB7C8CB-0843-4239-9044-DBF34DC2D882}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -432,8 +432,8 @@
   </sheetPr>
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1038,7 +1038,7 @@
         <v>24</v>
       </c>
       <c r="C29" s="2">
-        <f t="shared" si="1"/>
+        <f>POWER(2, B29)</f>
         <v>16777216</v>
       </c>
       <c r="D29" s="2">
@@ -1311,7 +1311,7 @@
         <v>37</v>
       </c>
       <c r="C42" s="2">
-        <f t="shared" si="1"/>
+        <f>POWER(2, B42)</f>
         <v>137438953472</v>
       </c>
       <c r="D42" s="2">

</xml_diff>

<commit_message>
pbrtのnextfloatよりも、Practically Accurate Floating-Point Mathのorderedのほうが直観的なので、こっちにする
</commit_message>
<xml_diff>
--- a/docs/ULP.xlsx
+++ b/docs/ULP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ushio\Documents\RayTracing\of_v0.10.1_vs2017_release\apps\with_ogaki\study\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{756BE9C9-511C-4C9C-AB5B-118D9C7C758A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A6B0E3-6E0D-42A0-A7C7-CDEAE524D5A1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="232" yWindow="4298" windowWidth="23873" windowHeight="15187" xr2:uid="{ECB7C8CB-0843-4239-9044-DBF34DC2D882}"/>
+    <workbookView xWindow="-75" yWindow="3188" windowWidth="23872" windowHeight="15187" xr2:uid="{ECB7C8CB-0843-4239-9044-DBF34DC2D882}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>E</t>
   </si>
@@ -47,13 +47,17 @@
   <si>
     <t>E-127</t>
   </si>
+  <si>
+    <t>誤差があるので、あとでちゃんとプロットする</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000000000000000000000000"/>
+    <numFmt numFmtId="165" formatCode="0.000000000000000000000000000000"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -106,13 +110,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -430,10 +435,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -442,10 +447,11 @@
     <col min="2" max="2" width="16.3984375" customWidth="1"/>
     <col min="3" max="3" width="18.86328125" customWidth="1"/>
     <col min="4" max="4" width="21.3984375" customWidth="1"/>
-    <col min="5" max="5" width="43.46484375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="45.73046875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="42.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -462,7 +468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>124</v>
       </c>
@@ -483,7 +489,7 @@
         <v>1.4901161193847656E-8</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>125</v>
       </c>
@@ -504,7 +510,7 @@
         <v>2.9802322387695313E-8</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>126</v>
       </c>
@@ -525,7 +531,7 @@
         <v>5.9604644775390625E-8</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>127</v>
       </c>
@@ -542,11 +548,14 @@
         <v>2</v>
       </c>
       <c r="E5" s="3">
-        <f t="shared" si="3"/>
+        <f>POWER(2, A5-23-127)</f>
         <v>1.1920928955078125E-7</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
         <v>128</v>
       </c>
@@ -567,7 +576,7 @@
         <v>2.384185791015625E-7</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" s="2">
         <v>129</v>
       </c>
@@ -584,11 +593,11 @@
         <v>8</v>
       </c>
       <c r="E7" s="3">
-        <f t="shared" si="3"/>
+        <f>POWER(2, A7-23-127)</f>
         <v>4.76837158203125E-7</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:6">
       <c r="A8" s="2">
         <v>130</v>
       </c>
@@ -609,7 +618,7 @@
         <v>9.5367431640625E-7</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" s="2">
         <v>131</v>
       </c>
@@ -630,7 +639,7 @@
         <v>1.9073486328125E-6</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10" s="2">
         <v>132</v>
       </c>
@@ -651,7 +660,7 @@
         <v>3.814697265625E-6</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11" s="2">
         <v>133</v>
       </c>
@@ -672,7 +681,7 @@
         <v>7.62939453125E-6</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
       <c r="A12" s="2">
         <v>134</v>
       </c>
@@ -693,7 +702,7 @@
         <v>1.52587890625E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="A13" s="2">
         <v>135</v>
       </c>
@@ -714,7 +723,7 @@
         <v>3.0517578125E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14" s="2">
         <v>136</v>
       </c>
@@ -735,7 +744,7 @@
         <v>6.103515625E-5</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6">
       <c r="A15" s="2">
         <v>137</v>
       </c>
@@ -756,7 +765,7 @@
         <v>1.220703125E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:6">
       <c r="A16" s="2">
         <v>138</v>
       </c>

</xml_diff>